<commit_message>
Novo módulos Indicadores VAAA
</commit_message>
<xml_diff>
--- a/IRD/ODS/VAI_VAM_VAV.xlsx
+++ b/IRD/ODS/VAI_VAM_VAV.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paulo\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Paulo\Documents\DGE\DGE\IRD\ODS\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -365,8 +365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection sqref="A1:D37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,6 +548,9 @@
       <c r="B19" s="1">
         <v>43252</v>
       </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
       <c r="D19">
         <v>6.93</v>
       </c>

</xml_diff>